<commit_message>
Atualização documentação Tabela LN
</commit_message>
<xml_diff>
--- a/Documentação/Tabelas_LN/znfmd630-TMS Ordens de Frete.xlsx
+++ b/Documentação/Tabelas_LN/znfmd630-TMS Ordens de Frete.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="525" windowWidth="19815" windowHeight="7365"/>
+    <workbookView xWindow="630" yWindow="810" windowWidth="19575" windowHeight="7080"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -327,7 +327,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="248">
   <si>
     <t/>
   </si>
@@ -359,13 +359,13 @@
     <t>VRC</t>
   </si>
   <si>
-    <t>Nº do campo</t>
+    <t>Nº seq</t>
   </si>
   <si>
     <t>Field</t>
   </si>
   <si>
-    <t>Comb.</t>
+    <t>Campo combinado</t>
   </si>
   <si>
     <t>Domínio</t>
@@ -380,7 +380,7 @@
     <t>Byte</t>
   </si>
   <si>
-    <t>Integer</t>
+    <t>Inteiro</t>
   </si>
   <si>
     <t>Long</t>
@@ -395,31 +395,31 @@
     <t>String</t>
   </si>
   <si>
-    <t>Enumerated</t>
-  </si>
-  <si>
-    <t>Set</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Text</t>
+    <t>Enumerado</t>
+  </si>
+  <si>
+    <t>Conjunto</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Texto</t>
   </si>
   <si>
     <t>Multibyte String</t>
   </si>
   <si>
-    <t>UTC Date/Time</t>
+    <t>Data/Hora UTC</t>
   </si>
   <si>
     <t>Raw</t>
   </si>
   <si>
-    <t>Binary Large Object</t>
-  </si>
-  <si>
-    <t>Comprimento</t>
+    <t>Objeto binário grande</t>
+  </si>
+  <si>
+    <t>Comp</t>
   </si>
   <si>
     <t>Related Label/Description</t>
@@ -731,13 +731,13 @@
     <t>stat.c</t>
   </si>
   <si>
-    <t>ibd.sepr</t>
-  </si>
-  <si>
-    <t>znfmd630.stat.c</t>
-  </si>
-  <si>
-    <t>Status (Fechada)</t>
+    <t>fmd.stof.c</t>
+  </si>
+  <si>
+    <t>znfmd200.stat.c</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
   <si>
     <t>ulog.c</t>
@@ -800,10 +800,10 @@
     <t>mcs.fdtc.l</t>
   </si>
   <si>
-    <t>znfmd630.fdtc.c</t>
-  </si>
-  <si>
-    <t>Cód.Tipo Documento Fiscal</t>
+    <t>sls.obsoleto.c</t>
+  </si>
+  <si>
+    <t>Obsoleto</t>
   </si>
   <si>
     <t>rfdt.c</t>
@@ -966,6 +966,111 @@
   </si>
   <si>
     <t>Referência Fiscal de Conciliação</t>
+  </si>
+  <si>
+    <t>vllq.c</t>
+  </si>
+  <si>
+    <t>copo.c</t>
+  </si>
+  <si>
+    <t>znsls401.copo.c</t>
+  </si>
+  <si>
+    <t>Coleta ou Postagem</t>
+  </si>
+  <si>
+    <t>frpe.c</t>
+  </si>
+  <si>
+    <t>znfmd630.frpe.c</t>
+  </si>
+  <si>
+    <t>Frete Peso</t>
+  </si>
+  <si>
+    <t>dtco.c</t>
+  </si>
+  <si>
+    <t>znfmd630.dtco.c</t>
+  </si>
+  <si>
+    <t>Data Corrigida</t>
+  </si>
+  <si>
+    <t>advc.c</t>
+  </si>
+  <si>
+    <t>znfmd630.advc.c</t>
+  </si>
+  <si>
+    <t>Ad Valorem Calculado</t>
+  </si>
+  <si>
+    <t>pedc.c</t>
+  </si>
+  <si>
+    <t>znfmd630.pedc.c</t>
+  </si>
+  <si>
+    <t>Pedágio Calculado</t>
+  </si>
+  <si>
+    <t>reet.c</t>
+  </si>
+  <si>
+    <t>znfmd630.reet.c</t>
+  </si>
+  <si>
+    <t>Reentrega Gerada</t>
+  </si>
+  <si>
+    <t>sqrt.c</t>
+  </si>
+  <si>
+    <t>mcs.long</t>
+  </si>
+  <si>
+    <t>znfmd630.sqrt.c</t>
+  </si>
+  <si>
+    <t>Sequencial Reentrega</t>
+  </si>
+  <si>
+    <t>rcal.c</t>
+  </si>
+  <si>
+    <t>znfmd630.rcal.c</t>
+  </si>
+  <si>
+    <t>Recalculado</t>
+  </si>
+  <si>
+    <t>dtrc.c</t>
+  </si>
+  <si>
+    <t>znfmd630.dtrc.c</t>
+  </si>
+  <si>
+    <t>Data do Recalculo</t>
+  </si>
+  <si>
+    <t>udap.c</t>
+  </si>
+  <si>
+    <t>znfmd630.udap.c</t>
+  </si>
+  <si>
+    <t>Última Data Acompanhar Pedido</t>
+  </si>
+  <si>
+    <t>dtpe.c</t>
+  </si>
+  <si>
+    <t>znfmd630.dtpe.c</t>
+  </si>
+  <si>
+    <t>Data Prevista de entrega</t>
   </si>
 </sst>
 </file>
@@ -1335,11 +1440,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R58"/>
+  <dimension ref="A1:R70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1352,13 +1457,13 @@
     <col min="7" max="7" width="3" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="21.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="34.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="9.140625" style="4"/>
@@ -2914,16 +3019,16 @@
         <v>8</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>134</v>
       </c>
       <c r="O28" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P28" s="4">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="Q28" s="4" t="s">
         <v>135</v>
@@ -4576,13 +4681,685 @@
         <v>212</v>
       </c>
     </row>
+    <row r="59" spans="1:18">
+      <c r="A59" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I59" s="4">
+        <v>0</v>
+      </c>
+      <c r="J59" s="4">
+        <v>58</v>
+      </c>
+      <c r="K59" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="L59" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M59" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N59" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="O59" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P59" s="4">
+        <v>19</v>
+      </c>
+      <c r="Q59" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="R59" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18">
+      <c r="A60" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I60" s="4">
+        <v>0</v>
+      </c>
+      <c r="J60" s="4">
+        <v>59</v>
+      </c>
+      <c r="K60" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="L60" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M60" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N60" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="O60" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P60" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q60" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="R60" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18">
+      <c r="A61" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I61" s="4">
+        <v>0</v>
+      </c>
+      <c r="J61" s="4">
+        <v>60</v>
+      </c>
+      <c r="K61" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="L61" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M61" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N61" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="O61" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P61" s="4">
+        <v>19</v>
+      </c>
+      <c r="Q61" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="R61" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18">
+      <c r="A62" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I62" s="4">
+        <v>0</v>
+      </c>
+      <c r="J62" s="4">
+        <v>61</v>
+      </c>
+      <c r="K62" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="L62" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M62" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N62" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="O62" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P62" s="4">
+        <v>22</v>
+      </c>
+      <c r="Q62" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="R62" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18">
+      <c r="A63" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I63" s="4">
+        <v>0</v>
+      </c>
+      <c r="J63" s="4">
+        <v>62</v>
+      </c>
+      <c r="K63" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="L63" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M63" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N63" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="O63" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P63" s="4">
+        <v>19</v>
+      </c>
+      <c r="Q63" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="R63" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18">
+      <c r="A64" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I64" s="4">
+        <v>0</v>
+      </c>
+      <c r="J64" s="4">
+        <v>63</v>
+      </c>
+      <c r="K64" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="L64" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M64" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N64" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="O64" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P64" s="4">
+        <v>19</v>
+      </c>
+      <c r="Q64" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="R64" s="4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18">
+      <c r="A65" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I65" s="4">
+        <v>0</v>
+      </c>
+      <c r="J65" s="4">
+        <v>64</v>
+      </c>
+      <c r="K65" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="L65" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M65" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N65" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="O65" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P65" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q65" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="R65" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18">
+      <c r="A66" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I66" s="4">
+        <v>0</v>
+      </c>
+      <c r="J66" s="4">
+        <v>65</v>
+      </c>
+      <c r="K66" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="L66" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M66" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N66" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="O66" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P66" s="4">
+        <v>10</v>
+      </c>
+      <c r="Q66" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="R66" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18">
+      <c r="A67" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I67" s="4">
+        <v>0</v>
+      </c>
+      <c r="J67" s="4">
+        <v>66</v>
+      </c>
+      <c r="K67" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="L67" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M67" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N67" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="O67" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P67" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q67" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="R67" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18">
+      <c r="A68" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I68" s="4">
+        <v>0</v>
+      </c>
+      <c r="J68" s="4">
+        <v>67</v>
+      </c>
+      <c r="K68" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="L68" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M68" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N68" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="O68" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P68" s="4">
+        <v>22</v>
+      </c>
+      <c r="Q68" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="R68" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18">
+      <c r="A69" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I69" s="4">
+        <v>0</v>
+      </c>
+      <c r="J69" s="4">
+        <v>68</v>
+      </c>
+      <c r="K69" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="L69" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M69" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N69" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="O69" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P69" s="4">
+        <v>22</v>
+      </c>
+      <c r="Q69" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="R69" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18">
+      <c r="A70" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I70" s="4">
+        <v>0</v>
+      </c>
+      <c r="J70" s="4">
+        <v>69</v>
+      </c>
+      <c r="K70" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="L70" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M70" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N70" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="O70" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P70" s="4">
+        <v>22</v>
+      </c>
+      <c r="Q70" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="R70" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048575">
+      <formula1>ttadv.type</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048575 E2:E1048575">
       <formula1>ttyeno</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048575">
-      <formula1>ttadv.type</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>